<commit_message>
Ya funciona el módulo del ECO.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -7,7 +7,10 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Stations_Mean" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Stations_Std" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Stations_CV" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,14 +19,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +51,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -345,14 +365,1169 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>StationID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Subregion</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Pontoon/Vessel/Place</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Lat</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Lon</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>DateUTC</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>startTimeUTC</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>endTimeUTC</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>timeStampUTC</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Overpasses</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ST01</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>12:34:00</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" s="2" t="n">
+        <v>43816.52361111111</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ST02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>13:02:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" s="2" t="n">
+        <v>43816.54305555556</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>{‘OLCI’:’S3B_OL_2_DER____20191217T130432_20191217T130732_20191226T142339_0179_033_209_3600_MAR_O_NT_002.SEN3’}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ST03</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" s="2" t="n">
+        <v>43816.57291666666</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>{‘OLI’:’’}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ST04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>14:31:00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" s="2" t="n">
+        <v>43816.60486111111</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ST05</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>15:02:00</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" s="2" t="n">
+        <v>43816.62638888889</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ST06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>15:36:00</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" s="2" t="n">
+        <v>43816.65</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ST07</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>16:12:00</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" s="2" t="n">
+        <v>43816.675</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ST08</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>16:35:00</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" s="2" t="n">
+        <v>43816.69097222222</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ST09</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>17:08:00</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" s="2" t="n">
+        <v>43816.71388888889</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ST10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>17:35:00</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" s="2" t="n">
+        <v>43816.73263888889</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ST11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>18:12:00</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" s="2" t="n">
+        <v>43816.75833333333</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>{‘VSNPP’:’V2019351180600’}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ST12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RdP</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CABA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Palermo (Pier)</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>-34.560833</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-58.398833</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>43816</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>18:50:00</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" s="2" t="n">
+        <v>43816.78472222222</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>StationID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>fl (CHL)</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>ntu (NTU)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>ST01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>6.833227868852466</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16.78652195121951</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ST02</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>6.689140000000005</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19.35518701298701</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>ST03</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6.655672972972981</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16.71418734177213</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>ST04</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6.657875342465761</v>
+      </c>
+      <c r="C6" t="n">
+        <v>17.03964324324324</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>ST05</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6.513193150684924</v>
+      </c>
+      <c r="C7" t="n">
+        <v>17.82110277777777</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ST06</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6.449998630136978</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17.95770684931506</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ST07</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>6.343149999999993</v>
+      </c>
+      <c r="C9" t="n">
+        <v>19.30708461538462</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>ST08</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6.410112698412695</v>
+      </c>
+      <c r="C10" t="n">
+        <v>24.16914594594595</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ST09</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7.712841558441561</v>
+      </c>
+      <c r="C11" t="n">
+        <v>20.83381818181819</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ST10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8.402247887323947</v>
+      </c>
+      <c r="C12" t="n">
+        <v>18.65070000000001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ST11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>8.989584507042261</v>
+      </c>
+      <c r="C13" t="n">
+        <v>18.93403513513512</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ST12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9.496557746478873</v>
+      </c>
+      <c r="C14" t="n">
+        <v>23.41481917808219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>StationID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>fl (CHL)</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>ntu (NTU)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>ST01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.208659964702865</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.8871340223047405</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ST02</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1929850337286373</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.227411491647817</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>ST03</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.04863522681072589</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2234014905759612</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>ST04</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.06926534683700439</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.6551386980791507</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>ST05</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.07880937325944455</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.403331978725464</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ST06</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.05725300208807745</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2544671318705726</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ST07</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.09163932654068943</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8033807956860318</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>ST08</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.09156396581706949</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.189841111050903</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ST09</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1706482310968581</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5149736152483098</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ST10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1316592342365644</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.2064960532310487</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ST11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.1350119155036614</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.3184572973813932</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ST12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.1336931333443142</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5397329753008351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>StationID</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>fl (CHL)</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>ntu (NTU)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>ST01</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3.053607587915932</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5.284799465206024</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ST02</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2.885050002371562</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.341511920418252</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>ST03</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.7307334210713379</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.336597981151232</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>ST04</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.040352113461947</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.844791165677334</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>ST05</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.209995948779087</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.263226825830349</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>ST06</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8876436317454159</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.417035783053104</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>ST07</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.444697453799603</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.161067357864414</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>ST08</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.428429890784027</v>
+      </c>
+      <c r="C10" t="n">
+        <v>13.19798853540357</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ST09</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.212520895234608</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.471815827296269</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ST10</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.566952510829776</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.107175887398589</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ST11</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.501870474635349</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.681930423750218</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ST12</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.407806248468134</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.305091366266286</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corregidos los errores de las columnas.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -994,10 +994,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.833227868852466</v>
+        <v>4.179417073170732</v>
       </c>
       <c r="C3" t="n">
-        <v>16.78652195121951</v>
+        <v>27.44548524590163</v>
       </c>
     </row>
     <row r="4">
@@ -1007,10 +1007,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.689140000000005</v>
+        <v>4.818949350649348</v>
       </c>
       <c r="C4" t="n">
-        <v>19.35518701298701</v>
+        <v>26.81466027397261</v>
       </c>
     </row>
     <row r="5">
@@ -1020,10 +1020,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6.655672972972981</v>
+        <v>4.161407594936702</v>
       </c>
       <c r="C5" t="n">
-        <v>16.71418734177213</v>
+        <v>26.73234054054054</v>
       </c>
     </row>
     <row r="6">
@@ -1033,10 +1033,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.657875342465761</v>
+        <v>4.24243783783784</v>
       </c>
       <c r="C6" t="n">
-        <v>17.03964324324324</v>
+        <v>26.74118630136986</v>
       </c>
     </row>
     <row r="7">
@@ -1046,10 +1046,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.513193150684924</v>
+        <v>4.426701449275361</v>
       </c>
       <c r="C7" t="n">
-        <v>17.82110277777777</v>
+        <v>26.16007397260275</v>
       </c>
     </row>
     <row r="8">
@@ -1059,10 +1059,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6.449998630136978</v>
+        <v>4.471012328767126</v>
       </c>
       <c r="C8" t="n">
-        <v>17.95770684931506</v>
+        <v>25.90625479452053</v>
       </c>
     </row>
     <row r="9">
@@ -1072,10 +1072,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.343149999999993</v>
+        <v>4.794501315789475</v>
       </c>
       <c r="C9" t="n">
-        <v>19.30708461538462</v>
+        <v>25.47709999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1085,10 +1085,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6.410112698412695</v>
+        <v>6.017502702702703</v>
       </c>
       <c r="C10" t="n">
-        <v>24.16914594594595</v>
+        <v>25.8668366197183</v>
       </c>
     </row>
     <row r="11">
@@ -1098,10 +1098,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7.712841558441561</v>
+        <v>5.187090909090905</v>
       </c>
       <c r="C11" t="n">
-        <v>20.83381818181819</v>
+        <v>30.97843116883117</v>
       </c>
     </row>
     <row r="12">
@@ -1111,10 +1111,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8.402247887323947</v>
+        <v>4.643550000000002</v>
       </c>
       <c r="C12" t="n">
-        <v>18.65070000000001</v>
+        <v>33.74741408450704</v>
       </c>
     </row>
     <row r="13">
@@ -1124,10 +1124,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8.989584507042261</v>
+        <v>4.714093243243243</v>
       </c>
       <c r="C13" t="n">
-        <v>18.93403513513512</v>
+        <v>36.10643661971831</v>
       </c>
     </row>
     <row r="14">
@@ -1137,10 +1137,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9.496557746478873</v>
+        <v>5.829694520547945</v>
       </c>
       <c r="C14" t="n">
-        <v>23.41481917808219</v>
+        <v>38.14268169014085</v>
       </c>
     </row>
   </sheetData>
@@ -1186,10 +1186,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.208659964702865</v>
+        <v>0.220873811131656</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8871340223047405</v>
+        <v>0.8380774200091998</v>
       </c>
     </row>
     <row r="4">
@@ -1199,10 +1199,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1929850337286373</v>
+        <v>0.3055942475103465</v>
       </c>
       <c r="C4" t="n">
-        <v>1.227411491647817</v>
+        <v>0.7171445489539521</v>
       </c>
     </row>
     <row r="5">
@@ -1212,10 +1212,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04863522681072589</v>
+        <v>0.0556212899013978</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2234014905759612</v>
+        <v>0.1953421465643332</v>
       </c>
     </row>
     <row r="6">
@@ -1225,10 +1225,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06926534683700439</v>
+        <v>0.1631128751985414</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6551386980791507</v>
+        <v>0.2782024968510989</v>
       </c>
     </row>
     <row r="7">
@@ -1238,10 +1238,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07880937325944455</v>
+        <v>0.08913679753244069</v>
       </c>
       <c r="C7" t="n">
-        <v>0.403331978725464</v>
+        <v>0.3165358352661047</v>
       </c>
     </row>
     <row r="8">
@@ -1251,10 +1251,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05725300208807745</v>
+        <v>0.063355844563346</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2544671318705726</v>
+        <v>0.2299552209073035</v>
       </c>
     </row>
     <row r="9">
@@ -1264,10 +1264,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09163932654068943</v>
+        <v>0.186891195079505</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8033807956860318</v>
+        <v>0.3680670150019801</v>
       </c>
     </row>
     <row r="10">
@@ -1277,10 +1277,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.09156396581706949</v>
+        <v>0.7941893168203027</v>
       </c>
       <c r="C10" t="n">
-        <v>3.189841111050903</v>
+        <v>0.4861261427241282</v>
       </c>
     </row>
     <row r="11">
@@ -1290,10 +1290,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1706482310968581</v>
+        <v>0.128215334067155</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5149736152483098</v>
+        <v>0.6854042626262595</v>
       </c>
     </row>
     <row r="12">
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1316592342365644</v>
+        <v>0.05141226591929673</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2064960532310487</v>
+        <v>0.5288059523373055</v>
       </c>
     </row>
     <row r="13">
@@ -1316,10 +1316,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1350119155036614</v>
+        <v>0.07928776846206127</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3184572973813932</v>
+        <v>0.5422719110344759</v>
       </c>
     </row>
     <row r="14">
@@ -1329,10 +1329,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1336931333443142</v>
+        <v>0.1343797850728497</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5397329753008351</v>
+        <v>0.5369750561671127</v>
       </c>
     </row>
   </sheetData>
@@ -1378,10 +1378,10 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>5.284799465206023</v>
+      </c>
+      <c r="C3" t="n">
         <v>3.053607587915932</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5.284799465206024</v>
       </c>
     </row>
     <row r="4">
@@ -1391,10 +1391,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.885050002371562</v>
+        <v>6.341511920418255</v>
       </c>
       <c r="C4" t="n">
-        <v>6.341511920418252</v>
+        <v>2.674449504959947</v>
       </c>
     </row>
     <row r="5">
@@ -1404,10 +1404,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7307334210713379</v>
+        <v>1.336597981151227</v>
       </c>
       <c r="C5" t="n">
-        <v>1.336597981151232</v>
+        <v>0.730733421071342</v>
       </c>
     </row>
     <row r="6">
@@ -1417,10 +1417,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.040352113461947</v>
+        <v>3.844791165677326</v>
       </c>
       <c r="C6" t="n">
-        <v>3.844791165677334</v>
+        <v>1.04035211346195</v>
       </c>
     </row>
     <row r="7">
@@ -1430,10 +1430,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.209995948779087</v>
+        <v>2.013616652350299</v>
       </c>
       <c r="C7" t="n">
-        <v>2.263226825830349</v>
+        <v>1.209995948779084</v>
       </c>
     </row>
     <row r="8">
@@ -1443,10 +1443,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8876436317454159</v>
+        <v>1.417035783053103</v>
       </c>
       <c r="C8" t="n">
-        <v>1.417035783053104</v>
+        <v>0.8876436317454179</v>
       </c>
     </row>
     <row r="9">
@@ -1456,10 +1456,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.444697453799603</v>
+        <v>3.898031990606118</v>
       </c>
       <c r="C9" t="n">
-        <v>4.161067357864414</v>
+        <v>1.444697453799609</v>
       </c>
     </row>
     <row r="10">
@@ -1469,10 +1469,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.428429890784027</v>
+        <v>13.19798853540357</v>
       </c>
       <c r="C10" t="n">
-        <v>13.19798853540357</v>
+        <v>1.879341296622077</v>
       </c>
     </row>
     <row r="11">
@@ -1482,10 +1482,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.212520895234608</v>
+        <v>2.471815827296271</v>
       </c>
       <c r="C11" t="n">
-        <v>2.471815827296269</v>
+        <v>2.212520895234606</v>
       </c>
     </row>
     <row r="12">
@@ -1495,10 +1495,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.566952510829776</v>
+        <v>1.107175887398579</v>
       </c>
       <c r="C12" t="n">
-        <v>1.107175887398589</v>
+        <v>1.566952510829779</v>
       </c>
     </row>
     <row r="13">
@@ -1508,10 +1508,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.501870474635349</v>
+        <v>1.681930423750214</v>
       </c>
       <c r="C13" t="n">
-        <v>1.681930423750218</v>
+        <v>1.501870474635352</v>
       </c>
     </row>
     <row r="14">
@@ -1521,10 +1521,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.407806248468134</v>
+        <v>2.305091366266291</v>
       </c>
       <c r="C14" t="n">
-        <v>2.305091366266286</v>
+        <v>1.407806248468132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en los nombres de las columnas.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -978,12 +978,12 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>fl (CHL)</t>
+          <t>chl (ug/l)</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ntu (NTU)</t>
+          <t>turbidity (NTU)</t>
         </is>
       </c>
     </row>
@@ -1170,12 +1170,12 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>fl (CHL)</t>
+          <t>chl (ug/l)</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ntu (NTU)</t>
+          <t>turbidity (NTU)</t>
         </is>
       </c>
     </row>
@@ -1362,12 +1362,12 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>fl (CHL)</t>
+          <t>chl (ug/l)</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ntu (NTU)</t>
+          <t>turbidity (NTU)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglado el bug de las fechas.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -10,7 +10,6 @@
     <sheet name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Stations_Mean" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Stations_Std" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Stations_CV" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1338,196 +1337,4 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A2:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>StationID</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>chl (ug/l)</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>turbidity (NTU)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>ST01</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5.284799465206023</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3.053607587915932</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>ST02</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>6.341511920418255</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2.674449504959947</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>ST03</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1.336597981151227</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.730733421071342</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>ST04</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3.844791165677326</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.04035211346195</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>ST05</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2.013616652350299</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1.209995948779084</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>ST06</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1.417035783053103</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.8876436317454179</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>ST07</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>3.898031990606118</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.444697453799609</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>ST08</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>13.19798853540357</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.879341296622077</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>ST09</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2.471815827296271</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2.212520895234606</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>ST10</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1.107175887398579</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.566952510829779</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>ST11</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1.681930423750214</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.501870474635352</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>ST12</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>2.305091366266291</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1.407806248468132</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Está hecha la eliminación de outliers.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,8 +21,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -61,22 +61,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -956,7 +956,7 @@
       <c r="L14" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1148,7 +1148,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1340,7 +1340,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1532,7 +1532,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1586,15 +1586,9 @@
       <c r="A2" s="3" t="n">
         <v>43816.50422453704</v>
       </c>
-      <c r="B2" t="n">
-        <v>994.7039999999998</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.227958193492945e-13</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.234496084757823e-14</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>19.19854285714286</v>
       </c>
@@ -1609,15 +1603,9 @@
       <c r="A3" s="3" t="n">
         <v>43816.50491898148</v>
       </c>
-      <c r="B3" t="n">
-        <v>994.7039999999998</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.192357613229151e-13</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.198705959993275e-14</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>16.45981666666667</v>
       </c>
@@ -1632,15 +1620,9 @@
       <c r="A4" s="3" t="n">
         <v>43816.50561342593</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.8200545454545455</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.185744188569892</v>
-      </c>
-      <c r="D4" t="n">
-        <v>144.5933316438908</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0</v>
       </c>
@@ -1654,13 +1636,13 @@
         <v>43816.50630787037</v>
       </c>
       <c r="B5" t="n">
-        <v>13.10425</v>
+        <v>25.40396</v>
       </c>
       <c r="C5" t="n">
-        <v>11.48009507091612</v>
+        <v>1.054276447617039</v>
       </c>
       <c r="D5" t="n">
-        <v>87.6058917596667</v>
+        <v>4.150047660353104</v>
       </c>
       <c r="E5" t="n">
         <v>2.599983333333333</v>
@@ -4153,13 +4135,13 @@
         <v>43816.58200231481</v>
       </c>
       <c r="B114" t="n">
-        <v>26.5742</v>
+        <v>26.49293333333334</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1990618664301798</v>
+        <v>0.1407579956284309</v>
       </c>
       <c r="D114" t="n">
-        <v>0.749079432043786</v>
+        <v>0.5313039287021101</v>
       </c>
       <c r="E114" t="n">
         <v>4.1276</v>
@@ -4646,10 +4628,10 @@
         <v>26.818</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1723926332532804</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>0.6428243465332255</v>
+        <v>0</v>
       </c>
       <c r="E136" t="n">
         <v>4.046666666666667</v>
@@ -5370,15 +5352,9 @@
       <c r="A168" s="3" t="n">
         <v>43816.61950231482</v>
       </c>
-      <c r="B168" t="n">
-        <v>0.4063333333333333</v>
-      </c>
-      <c r="C168" t="n">
-        <v>1.027147657350198</v>
-      </c>
-      <c r="D168" t="n">
-        <v>252.7844931952908</v>
-      </c>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
       <c r="E168" t="n">
         <v>0.008671428571428571</v>
       </c>
@@ -6996,13 +6972,13 @@
         <v>43816.66880787037</v>
       </c>
       <c r="B239" t="n">
-        <v>69.72680000000001</v>
+        <v>25.9647</v>
       </c>
       <c r="C239" t="n">
-        <v>75.79827866673492</v>
+        <v>0.1723926332532804</v>
       </c>
       <c r="D239" t="n">
-        <v>108.7075251793212</v>
+        <v>0.6639500292831438</v>
       </c>
       <c r="E239" t="n">
         <v>4.835766666666667</v>
@@ -11547,13 +11523,13 @@
         <v>43816.8083912037</v>
       </c>
       <c r="B440" t="n">
-        <v>20.86231428571429</v>
+        <v>39.08926666666667</v>
       </c>
       <c r="C440" t="n">
-        <v>19.5206815567002</v>
+        <v>0.372410651476745</v>
       </c>
       <c r="D440" t="n">
-        <v>93.5691088215808</v>
+        <v>0.9527184396997598</v>
       </c>
       <c r="E440" t="n">
         <v>2.982971428571428</v>
@@ -11569,15 +11545,9 @@
       <c r="A441" s="3" t="n">
         <v>43816.80908564815</v>
       </c>
-      <c r="B441" t="n">
-        <v>1.65784</v>
-      </c>
-      <c r="C441" t="n">
-        <v>2.217105993857758</v>
-      </c>
-      <c r="D441" t="n">
-        <v>133.7346181692901</v>
-      </c>
+      <c r="B441" t="inlineStr"/>
+      <c r="C441" t="inlineStr"/>
+      <c r="D441" t="inlineStr"/>
       <c r="E441" t="n">
         <v>0.015175</v>
       </c>
@@ -11592,12 +11562,8 @@
       <c r="A442" s="3" t="n">
         <v>43816.80978009259</v>
       </c>
-      <c r="B442" t="n">
-        <v>0</v>
-      </c>
-      <c r="C442" t="n">
-        <v>0</v>
-      </c>
+      <c r="B442" t="inlineStr"/>
+      <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="n">
         <v>0</v>
@@ -11611,12 +11577,8 @@
       <c r="A443" s="3" t="n">
         <v>43816.81047453704</v>
       </c>
-      <c r="B443" t="n">
-        <v>0</v>
-      </c>
-      <c r="C443" t="n">
-        <v>0</v>
-      </c>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="n">
         <v>0</v>
@@ -11630,12 +11592,8 @@
       <c r="A444" s="3" t="n">
         <v>43816.81116898148</v>
       </c>
-      <c r="B444" t="n">
-        <v>0</v>
-      </c>
-      <c r="C444" t="n">
-        <v>0</v>
-      </c>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr"/>
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="n">
         <v>0</v>
@@ -11649,15 +11607,9 @@
       <c r="A445" s="3" t="n">
         <v>43816.86603009259</v>
       </c>
-      <c r="B445" t="n">
-        <v>994.7040000000001</v>
-      </c>
-      <c r="C445" t="n">
-        <v>1.392373714442771e-13</v>
-      </c>
-      <c r="D445" t="n">
-        <v>1.399786986322334e-14</v>
-      </c>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+      <c r="D445" t="inlineStr"/>
       <c r="E445" t="n">
         <v>31.0177</v>
       </c>
@@ -11669,6 +11621,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego la comparación de los datos de las dos transferencias.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -1586,9 +1586,15 @@
       <c r="A2" s="3" t="n">
         <v>43816.50422453704</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>994.7039999999998</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.227958193492945e-13</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.234496084757823e-14</v>
+      </c>
       <c r="E2" t="n">
         <v>19.19854285714286</v>
       </c>
@@ -1603,9 +1609,15 @@
       <c r="A3" s="3" t="n">
         <v>43816.50491898148</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>994.7039999999998</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.192357613229151e-13</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.198705959993275e-14</v>
+      </c>
       <c r="E3" t="n">
         <v>16.45981666666667</v>
       </c>
@@ -1620,9 +1632,15 @@
       <c r="A4" s="3" t="n">
         <v>43816.50561342593</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>0.8200545454545455</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.185744188569892</v>
+      </c>
+      <c r="D4" t="n">
+        <v>144.5933316438908</v>
+      </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
@@ -1636,13 +1654,13 @@
         <v>43816.50630787037</v>
       </c>
       <c r="B5" t="n">
-        <v>25.40396</v>
+        <v>13.10425</v>
       </c>
       <c r="C5" t="n">
-        <v>1.054276447617039</v>
+        <v>11.48009507091612</v>
       </c>
       <c r="D5" t="n">
-        <v>4.150047660353104</v>
+        <v>87.6058917596667</v>
       </c>
       <c r="E5" t="n">
         <v>2.599983333333333</v>
@@ -4135,13 +4153,13 @@
         <v>43816.58200231481</v>
       </c>
       <c r="B114" t="n">
-        <v>26.49293333333334</v>
+        <v>26.5742</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1407579956284309</v>
+        <v>0.1990618664301798</v>
       </c>
       <c r="D114" t="n">
-        <v>0.5313039287021101</v>
+        <v>0.749079432043786</v>
       </c>
       <c r="E114" t="n">
         <v>4.1276</v>
@@ -4628,10 +4646,10 @@
         <v>26.818</v>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>0.1723926332532804</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>0.6428243465332255</v>
       </c>
       <c r="E136" t="n">
         <v>4.046666666666667</v>
@@ -5352,9 +5370,15 @@
       <c r="A168" s="3" t="n">
         <v>43816.61950231482</v>
       </c>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
-      <c r="D168" t="inlineStr"/>
+      <c r="B168" t="n">
+        <v>0.4063333333333333</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1.027147657350198</v>
+      </c>
+      <c r="D168" t="n">
+        <v>252.7844931952908</v>
+      </c>
       <c r="E168" t="n">
         <v>0.008671428571428571</v>
       </c>
@@ -6972,13 +6996,13 @@
         <v>43816.66880787037</v>
       </c>
       <c r="B239" t="n">
-        <v>25.9647</v>
+        <v>69.72680000000001</v>
       </c>
       <c r="C239" t="n">
-        <v>0.1723926332532804</v>
+        <v>75.79827866673492</v>
       </c>
       <c r="D239" t="n">
-        <v>0.6639500292831438</v>
+        <v>108.7075251793212</v>
       </c>
       <c r="E239" t="n">
         <v>4.835766666666667</v>
@@ -11523,13 +11547,13 @@
         <v>43816.8083912037</v>
       </c>
       <c r="B440" t="n">
-        <v>39.08926666666667</v>
+        <v>20.86231428571429</v>
       </c>
       <c r="C440" t="n">
-        <v>0.372410651476745</v>
+        <v>19.5206815567002</v>
       </c>
       <c r="D440" t="n">
-        <v>0.9527184396997598</v>
+        <v>93.5691088215808</v>
       </c>
       <c r="E440" t="n">
         <v>2.982971428571428</v>
@@ -11545,9 +11569,15 @@
       <c r="A441" s="3" t="n">
         <v>43816.80908564815</v>
       </c>
-      <c r="B441" t="inlineStr"/>
-      <c r="C441" t="inlineStr"/>
-      <c r="D441" t="inlineStr"/>
+      <c r="B441" t="n">
+        <v>1.65784</v>
+      </c>
+      <c r="C441" t="n">
+        <v>2.217105993857758</v>
+      </c>
+      <c r="D441" t="n">
+        <v>133.7346181692901</v>
+      </c>
       <c r="E441" t="n">
         <v>0.015175</v>
       </c>
@@ -11562,8 +11592,12 @@
       <c r="A442" s="3" t="n">
         <v>43816.80978009259</v>
       </c>
-      <c r="B442" t="inlineStr"/>
-      <c r="C442" t="inlineStr"/>
+      <c r="B442" t="n">
+        <v>0</v>
+      </c>
+      <c r="C442" t="n">
+        <v>0</v>
+      </c>
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="n">
         <v>0</v>
@@ -11577,8 +11611,12 @@
       <c r="A443" s="3" t="n">
         <v>43816.81047453704</v>
       </c>
-      <c r="B443" t="inlineStr"/>
-      <c r="C443" t="inlineStr"/>
+      <c r="B443" t="n">
+        <v>0</v>
+      </c>
+      <c r="C443" t="n">
+        <v>0</v>
+      </c>
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="n">
         <v>0</v>
@@ -11592,8 +11630,12 @@
       <c r="A444" s="3" t="n">
         <v>43816.81116898148</v>
       </c>
-      <c r="B444" t="inlineStr"/>
-      <c r="C444" t="inlineStr"/>
+      <c r="B444" t="n">
+        <v>0</v>
+      </c>
+      <c r="C444" t="n">
+        <v>0</v>
+      </c>
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="n">
         <v>0</v>
@@ -11607,9 +11649,15 @@
       <c r="A445" s="3" t="n">
         <v>43816.86603009259</v>
       </c>
-      <c r="B445" t="inlineStr"/>
-      <c r="C445" t="inlineStr"/>
-      <c r="D445" t="inlineStr"/>
+      <c r="B445" t="n">
+        <v>994.7040000000001</v>
+      </c>
+      <c r="C445" t="n">
+        <v>1.392373714442771e-13</v>
+      </c>
+      <c r="D445" t="n">
+        <v>1.399786986322334e-14</v>
+      </c>
       <c r="E445" t="n">
         <v>31.0177</v>
       </c>

</xml_diff>

<commit_message>
Últimas modificaciones sobre los ajustes de los datos suavizados y agrego el informe de junio.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191217_Muelle/ECO_FLNTUProcessed/RdP_20191217_ECO-FLNTU.xlsx
@@ -1586,15 +1586,9 @@
       <c r="A2" s="3" t="n">
         <v>43816.50422453704</v>
       </c>
-      <c r="B2" t="n">
-        <v>994.7039999999998</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.227958193492945e-13</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.234496084757823e-14</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>19.19854285714286</v>
       </c>
@@ -1609,15 +1603,9 @@
       <c r="A3" s="3" t="n">
         <v>43816.50491898148</v>
       </c>
-      <c r="B3" t="n">
-        <v>994.7039999999998</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.192357613229151e-13</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.198705959993275e-14</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
         <v>16.45981666666667</v>
       </c>
@@ -1632,15 +1620,9 @@
       <c r="A4" s="3" t="n">
         <v>43816.50561342593</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.8200545454545455</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.185744188569892</v>
-      </c>
-      <c r="D4" t="n">
-        <v>144.5933316438908</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0</v>
       </c>
@@ -1654,13 +1636,13 @@
         <v>43816.50630787037</v>
       </c>
       <c r="B5" t="n">
-        <v>13.10425</v>
+        <v>25.40396</v>
       </c>
       <c r="C5" t="n">
-        <v>11.48009507091612</v>
+        <v>1.054276447617039</v>
       </c>
       <c r="D5" t="n">
-        <v>87.6058917596667</v>
+        <v>4.150047660353104</v>
       </c>
       <c r="E5" t="n">
         <v>2.599983333333333</v>
@@ -4153,13 +4135,13 @@
         <v>43816.58200231481</v>
       </c>
       <c r="B114" t="n">
-        <v>26.5742</v>
+        <v>26.49293333333334</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1990618664301798</v>
+        <v>0.1407579956284309</v>
       </c>
       <c r="D114" t="n">
-        <v>0.749079432043786</v>
+        <v>0.5313039287021101</v>
       </c>
       <c r="E114" t="n">
         <v>4.1276</v>
@@ -4646,10 +4628,10 @@
         <v>26.818</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1723926332532804</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>0.6428243465332255</v>
+        <v>0</v>
       </c>
       <c r="E136" t="n">
         <v>4.046666666666667</v>
@@ -5370,15 +5352,9 @@
       <c r="A168" s="3" t="n">
         <v>43816.61950231482</v>
       </c>
-      <c r="B168" t="n">
-        <v>0.4063333333333333</v>
-      </c>
-      <c r="C168" t="n">
-        <v>1.027147657350198</v>
-      </c>
-      <c r="D168" t="n">
-        <v>252.7844931952908</v>
-      </c>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
       <c r="E168" t="n">
         <v>0.008671428571428571</v>
       </c>
@@ -6996,13 +6972,13 @@
         <v>43816.66880787037</v>
       </c>
       <c r="B239" t="n">
-        <v>69.72680000000001</v>
+        <v>25.9647</v>
       </c>
       <c r="C239" t="n">
-        <v>75.79827866673492</v>
+        <v>0.1723926332532804</v>
       </c>
       <c r="D239" t="n">
-        <v>108.7075251793212</v>
+        <v>0.6639500292831438</v>
       </c>
       <c r="E239" t="n">
         <v>4.835766666666667</v>
@@ -11547,13 +11523,13 @@
         <v>43816.8083912037</v>
       </c>
       <c r="B440" t="n">
-        <v>20.86231428571429</v>
+        <v>39.08926666666667</v>
       </c>
       <c r="C440" t="n">
-        <v>19.5206815567002</v>
+        <v>0.372410651476745</v>
       </c>
       <c r="D440" t="n">
-        <v>93.5691088215808</v>
+        <v>0.9527184396997598</v>
       </c>
       <c r="E440" t="n">
         <v>2.982971428571428</v>
@@ -11569,15 +11545,9 @@
       <c r="A441" s="3" t="n">
         <v>43816.80908564815</v>
       </c>
-      <c r="B441" t="n">
-        <v>1.65784</v>
-      </c>
-      <c r="C441" t="n">
-        <v>2.217105993857758</v>
-      </c>
-      <c r="D441" t="n">
-        <v>133.7346181692901</v>
-      </c>
+      <c r="B441" t="inlineStr"/>
+      <c r="C441" t="inlineStr"/>
+      <c r="D441" t="inlineStr"/>
       <c r="E441" t="n">
         <v>0.015175</v>
       </c>
@@ -11592,12 +11562,8 @@
       <c r="A442" s="3" t="n">
         <v>43816.80978009259</v>
       </c>
-      <c r="B442" t="n">
-        <v>0</v>
-      </c>
-      <c r="C442" t="n">
-        <v>0</v>
-      </c>
+      <c r="B442" t="inlineStr"/>
+      <c r="C442" t="inlineStr"/>
       <c r="D442" t="inlineStr"/>
       <c r="E442" t="n">
         <v>0</v>
@@ -11611,12 +11577,8 @@
       <c r="A443" s="3" t="n">
         <v>43816.81047453704</v>
       </c>
-      <c r="B443" t="n">
-        <v>0</v>
-      </c>
-      <c r="C443" t="n">
-        <v>0</v>
-      </c>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr"/>
       <c r="D443" t="inlineStr"/>
       <c r="E443" t="n">
         <v>0</v>
@@ -11630,12 +11592,8 @@
       <c r="A444" s="3" t="n">
         <v>43816.81116898148</v>
       </c>
-      <c r="B444" t="n">
-        <v>0</v>
-      </c>
-      <c r="C444" t="n">
-        <v>0</v>
-      </c>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr"/>
       <c r="D444" t="inlineStr"/>
       <c r="E444" t="n">
         <v>0</v>
@@ -11649,15 +11607,9 @@
       <c r="A445" s="3" t="n">
         <v>43816.86603009259</v>
       </c>
-      <c r="B445" t="n">
-        <v>994.7040000000001</v>
-      </c>
-      <c r="C445" t="n">
-        <v>1.392373714442771e-13</v>
-      </c>
-      <c r="D445" t="n">
-        <v>1.399786986322334e-14</v>
-      </c>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+      <c r="D445" t="inlineStr"/>
       <c r="E445" t="n">
         <v>31.0177</v>
       </c>

</xml_diff>